<commit_message>
Communication Matrix ver 1.2
See changes on "Version & History Tab"
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Version &amp; History" sheetId="2" r:id="rId1"/>
+    <sheet name="CommunicationMatrix" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Munka1!$A$2:$J$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CommunicationMatrix!$A$2:$J$10</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t>Signal Name</t>
   </si>
@@ -43,15 +44,9 @@
     <t>Input</t>
   </si>
   <si>
-    <t>Wheel angle</t>
-  </si>
-  <si>
     <t>°</t>
   </si>
   <si>
-    <t>Switch position</t>
-  </si>
-  <si>
     <t>Physical values</t>
   </si>
   <si>
@@ -79,15 +74,9 @@
     <t>Car angle</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Communication matrix for the UniDebAutomatedCar project</t>
   </si>
   <si>
-    <t>Driver</t>
-  </si>
-  <si>
     <t>Signal ID</t>
   </si>
   <si>
@@ -106,18 +95,96 @@
     <t>PowertrainSystem</t>
   </si>
   <si>
-    <t>FORWARD: 1
-BACKWARD: 0</t>
-  </si>
-  <si>
     <t>These signals go directly to the AutomatedCar</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>NONE: 0
+RIGHT: 1
+LEFT: 2
+EMERGENCY: 3</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>Steering Wheel Angle</t>
+  </si>
+  <si>
+    <t>Gear Position</t>
+  </si>
+  <si>
+    <t>PowertrainSystem
+Instrument Cluster</t>
+  </si>
+  <si>
+    <t>Brake pedal position</t>
+  </si>
+  <si>
+    <t>D
+N
+R
+P</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Additional information</t>
+  </si>
+  <si>
+    <t>Change history</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Detailed description of change</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <t>Krisztian Holman</t>
+  </si>
+  <si>
+    <t>Tamas Miklos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Release </t>
+  </si>
+  <si>
+    <t>New signals:
+- Indicator
+- Brake pedal position
+Renamed:
+Wheel Angle -&gt; Steering Wheel Angle
+Switch Position -&gt; Gear Position
+Signal Ids have been changed!</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Draft version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +223,42 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="CorpoS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="CorpoS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="CorpoS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -220,17 +323,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -251,11 +343,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -264,7 +371,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -272,31 +378,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,7 +448,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -324,7 +464,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -610,16 +750,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" ht="22.5" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24" customHeight="1">
+      <c r="A5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="24">
+        <v>42797</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="135">
+      <c r="A6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="24">
+        <v>42801</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" customHeight="1">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" ht="24" customHeight="1">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:5" ht="24" customHeight="1">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="17.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
@@ -627,54 +884,57 @@
     <col min="7" max="7" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="5" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-    </row>
-    <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+    <row r="1" spans="1:11" ht="21">
+      <c r="A1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:11" ht="12.75">
+      <c r="A2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="20"/>
+      <c r="K2" s="28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="12.75">
+      <c r="A3" s="29"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
@@ -682,233 +942,281 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="5">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>5</v>
+      <c r="B4" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
-        <v>100</v>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>8</v>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>-60</v>
-      </c>
-      <c r="D5" s="1">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1">
       <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>29</v>
+      <c r="B6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>360</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="45">
       <c r="A7" s="5">
         <v>3</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>16</v>
+      <c r="B7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" ht="22.5">
       <c r="A8" s="5">
         <v>4</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>17</v>
+      <c r="B8" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
+      <c r="D8" s="1">
+        <v>100</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="22.5">
       <c r="A9" s="5">
         <v>5</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1">
         <v>0</v>
       </c>
-      <c r="D9" s="2">
-        <v>360</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>18</v>
+      <c r="F9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J9" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="22.5">
       <c r="A10" s="5">
         <v>6</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-720</v>
+      </c>
+      <c r="D10" s="1">
+        <v>720</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45">
       <c r="A11" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>8</v>
+      <c r="B11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="K4:K6"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="I2:I3"/>
@@ -916,6 +1224,7 @@
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CommunicationMatrix updated to 1.2 and UniDebAutomCar2017-1_Requirements updated by Team1
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -614,7 +614,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -661,10 +661,6 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -823,7 +819,7 @@
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -831,7 +827,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.6"/>
   </cols>
@@ -914,23 +910,23 @@
       <c r="D7" s="8" t="n">
         <v>42802</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -959,479 +955,479 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="17" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="15" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="20.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="15" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="75.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="17" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="16" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="14" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="14" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="14" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="16" width="75.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="16" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="19" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" s="23" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="22" t="s">
+    <row r="3" s="22" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="n">
+      <c r="A4" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="17" t="n">
+      <c r="C4" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="17" t="n">
+      <c r="E4" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="15" t="s">
+      <c r="G4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="n">
+      <c r="A5" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="17" t="n">
+      <c r="C5" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="17" t="n">
+      <c r="E5" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="25"/>
-    </row>
-    <row r="6" s="23" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="n">
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" s="22" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="26" t="n">
+      <c r="C6" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="26" t="n">
+      <c r="D6" s="25" t="n">
         <v>360</v>
       </c>
-      <c r="E6" s="26" t="n">
+      <c r="E6" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="15" t="s">
+      <c r="G6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="25"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="n">
+      <c r="A7" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="27" t="s">
+      <c r="C7" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="26"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="n">
+      <c r="A8" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="17" t="n">
+      <c r="C8" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="17" t="n">
+      <c r="D8" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="E8" s="17" t="n">
+      <c r="E8" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="n">
+      <c r="A9" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="17" t="n">
+      <c r="C9" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="17" t="n">
+      <c r="D9" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="E9" s="17" t="n">
+      <c r="E9" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="15" t="s">
+      <c r="G9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="n">
+      <c r="A10" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="17" t="n">
+      <c r="C10" s="16" t="n">
         <v>-720</v>
       </c>
-      <c r="D10" s="17" t="n">
+      <c r="D10" s="16" t="n">
         <v>720</v>
       </c>
-      <c r="E10" s="17" t="n">
+      <c r="E10" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="15" t="s">
+      <c r="G10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
+      <c r="A11" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="27" t="s">
+      <c r="C11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="n">
+      <c r="A12" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="17" t="n">
+      <c r="C12" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="17" t="n">
+      <c r="D12" s="16" t="n">
         <v>120</v>
       </c>
-      <c r="E12" s="17" t="n">
+      <c r="E12" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="15" t="s">
+      <c r="G12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="n">
+      <c r="A13" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="17" t="n">
+      <c r="C13" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="17" t="n">
+      <c r="D13" s="16" t="n">
         <v>9000</v>
       </c>
-      <c r="E13" s="17" t="n">
+      <c r="E13" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="15" t="s">
+      <c r="G13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="n">
+      <c r="A14" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="27" t="s">
+      <c r="C14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="n">
+      <c r="A15" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="27" t="s">
+      <c r="C15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="16" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed accidentally added future feature informations
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
   <si>
     <t>Change history</t>
   </si>
@@ -246,28 +246,6 @@
     <t>This signal will set the visual indicator for the headlight state</t>
   </si>
   <si>
-    <t>ACC</t>
-  </si>
-  <si>
-    <t>TSR</t>
-  </si>
-  <si>
-    <t>PP</t>
-  </si>
-  <si>
-    <t>LKS</t>
-  </si>
-  <si>
-    <t>ENABLE: TRUE
-DISABLE: FALSE</t>
-  </si>
-  <si>
-    <t>DISABLE: 0
-ENABLE: 1
-Set wehicle speed: 2
-set safety distance: 3</t>
-  </si>
-  <si>
     <t>V1.3</t>
   </si>
   <si>
@@ -276,6 +254,12 @@
   <si>
     <t>Added new signals for ACC, TSR, LKS and PP.
 Edited resolutions of gas pedal, brake pedal and steering wheel based on the requirements documentation.</t>
+  </si>
+  <si>
+    <t>V1.4</t>
+  </si>
+  <si>
+    <t>Realized that I've put infomations about some future features, so temporarily removed them from the communications matrix.</t>
   </si>
 </sst>
 </file>
@@ -468,26 +452,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -519,13 +485,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -544,6 +504,24 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -924,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -939,110 +917,120 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="7">
         <v>42797</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="135">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="7">
         <v>42801</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="135">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="7">
         <v>42802</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="24" customHeight="1">
-      <c r="A8" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="A8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="7">
         <v>42802</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="A9" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="7">
+        <v>42802</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1057,615 +1045,503 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK19"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="22" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="21" style="20" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="20" customWidth="1"/>
-    <col min="11" max="11" width="75.85546875" style="22" customWidth="1"/>
-    <col min="12" max="1025" width="9.140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="14" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="21" style="12" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="75.85546875" style="14" customWidth="1"/>
+    <col min="12" max="1025" width="9.140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="25" customFormat="1" ht="12.75">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="24" t="s">
+    <row r="3" spans="1:11" s="17" customFormat="1" ht="12.75">
+      <c r="A3" s="23"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="20">
+      <c r="A4" s="12">
         <v>0</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="14">
         <v>0</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="14">
         <v>1</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="20" t="s">
+      <c r="G4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="20">
+      <c r="A5" s="12">
         <v>1</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="14">
         <v>0</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="14">
         <v>1</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" s="25" customFormat="1" ht="11.25">
-      <c r="A6" s="20">
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" s="17" customFormat="1" ht="11.25">
+      <c r="A6" s="12">
         <v>2</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="19">
         <v>0</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="19">
         <v>360</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="19">
         <v>1</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="20" t="s">
+      <c r="G6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" ht="45.75">
-      <c r="A7" s="20">
+      <c r="A7" s="12">
         <v>3</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="28" t="s">
+      <c r="C7" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="27"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" ht="23.25">
-      <c r="A8" s="20">
+      <c r="A8" s="12">
         <v>4</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="14">
         <v>0</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="14">
         <v>100</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="14">
         <v>100</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="20" t="s">
+      <c r="G8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="23.25">
-      <c r="A9" s="20">
+      <c r="A9" s="12">
         <v>5</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="14">
         <v>0</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="14">
         <v>100</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="14">
         <v>100</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="20" t="s">
+      <c r="G9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="23.25">
-      <c r="A10" s="20">
+      <c r="A10" s="12">
         <v>6</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="14">
         <v>-720</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="14">
         <v>720</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="14">
         <v>15</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="20" t="s">
+      <c r="G10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45.75">
-      <c r="A11" s="20">
+      <c r="A11" s="12">
         <v>7</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="28" t="s">
+      <c r="C11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="23.25">
-      <c r="A12" s="20">
+      <c r="A12" s="12">
         <v>8</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="14">
         <v>0</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="14">
         <v>120</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="14">
         <v>1</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="20" t="s">
+      <c r="G12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="23.25">
-      <c r="A13" s="20">
+      <c r="A13" s="12">
         <v>9</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="14">
         <v>0</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="14">
         <v>9000</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="14">
         <v>1</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="20" t="s">
+      <c r="G13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="K13" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45.75">
-      <c r="A14" s="20">
+      <c r="A14" s="12">
         <v>10</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="28" t="s">
+      <c r="C14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="K14" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="23.25">
-      <c r="A15" s="20">
+      <c r="A15" s="12">
         <v>11</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="28" t="s">
+      <c r="C15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="K15" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="45.75">
-      <c r="A16" s="20">
-        <v>12</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J16" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="23.25">
-      <c r="A17" s="20">
-        <v>13</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="45.75">
-      <c r="A18" s="20">
-        <v>14</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="23.25">
-      <c r="A19" s="20">
-        <v>15</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" s="28" t="s">
-        <v>45</v>
-      </c>
+    <row r="16" spans="1:11">
+      <c r="G16" s="20"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="7:10">
+      <c r="G17" s="20"/>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="7:10">
+      <c r="G18" s="20"/>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="7:10">
+      <c r="G19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Comm matrix freeze #1 - fixed Communication matrix based on the ticket's comments
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>Change history</t>
   </si>
@@ -224,18 +224,6 @@
     <t>This signal will set the visual indicator for the motor rpm</t>
   </si>
   <si>
-    <t>Turn Signals</t>
-  </si>
-  <si>
-    <t>NONE: 00
-RIGHT: 01
-LEFT: 10
-EMERGENCY: 11</t>
-  </si>
-  <si>
-    <t>First two bits of a byte (01 – right, 10 – left, 11 - Emergency Indicator) This representation was demanded by the customer!</t>
-  </si>
-  <si>
     <t>Headlight</t>
   </si>
   <si>
@@ -260,6 +248,12 @@
   </si>
   <si>
     <t>Realized that I've put infomations about some future features, so temporarily removed them from the communications matrix.</t>
+  </si>
+  <si>
+    <t>V1.5</t>
+  </si>
+  <si>
+    <t>Fixed both accelerator and brake pedal resolutions and also fixed the steering wheel angle resolution.</t>
   </si>
 </sst>
 </file>
@@ -900,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1000,13 +994,13 @@
     </row>
     <row r="8" spans="1:5" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D8" s="7">
         <v>42802</v>
@@ -1017,18 +1011,35 @@
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" s="7">
         <v>42802</v>
       </c>
       <c r="E9" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="25.5">
+      <c r="A10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="7">
+        <v>42803</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1037,16 +1048,16 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK19"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1276,7 +1287,7 @@
         <v>100</v>
       </c>
       <c r="E8" s="14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>47</v>
@@ -1308,7 +1319,7 @@
         <v>100</v>
       </c>
       <c r="E9" s="14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>47</v>
@@ -1340,7 +1351,7 @@
         <v>720</v>
       </c>
       <c r="E10" s="14">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>40</v>
@@ -1457,7 +1468,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45.75">
+    <row r="14" spans="1:11" ht="23.25">
       <c r="A14" s="12">
         <v>10</v>
       </c>
@@ -1492,40 +1503,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="23.25">
-      <c r="A15" s="12">
-        <v>11</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="14" t="s">
-        <v>63</v>
-      </c>
+    <row r="15" spans="1:11">
+      <c r="G15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:11">
       <c r="G16" s="20"/>
@@ -1538,10 +1518,6 @@
     <row r="18" spans="7:10">
       <c r="G18" s="20"/>
       <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="7:10">
-      <c r="G19" s="20"/>
-      <c r="J19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Changed the "Type" and "Receiver" columns in the ComMatrix.xlsx (Vehicle Speed and Motor RPM)
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -843,7 +843,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
@@ -1002,23 +1002,23 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="16" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="16" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="14" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="14" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="14" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="14" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="16" width="75.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="16" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="16" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="16" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
CommMatrix v1.8 - Review findings fixed
https://trello.com/c/5sJGWGHP/11-comm-matrix-freeze-1
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\school\bosch\gitrepo\UniDebAutomatedCar\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GH\UniDeb2017-1\UniDebAutomatedCar\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version &amp; History" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
   <si>
     <t>Change history</t>
   </si>
@@ -231,12 +231,6 @@
     <t>Gear Position</t>
   </si>
   <si>
-    <t>D
-N
-R
-P</t>
-  </si>
-  <si>
     <t>Vehicle Speed</t>
   </si>
   <si>
@@ -261,10 +255,6 @@
     <t>Headlight</t>
   </si>
   <si>
-    <t>ON: TRUE
-OFF: FALSE</t>
-  </si>
-  <si>
     <t>This signal will set the visual indicator for the headlight state</t>
   </si>
   <si>
@@ -274,7 +264,29 @@
     <t>Freezed the communication matrix.</t>
   </si>
   <si>
-    <t>Final version</t>
+    <t>Working version for Sprint #1</t>
+  </si>
+  <si>
+    <t>V1.8</t>
+  </si>
+  <si>
+    <t>D: 0
+N: 1
+R: 2
+P: 3</t>
+  </si>
+  <si>
+    <t>ON: 1
+OFF: 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instrument Cluster has been removed as receiver for the following signals:
+- Gas pedal position
+- Brake pedal position
+Logical valueset specified for:
+- Gear position
+- Headlight
+</t>
   </si>
 </sst>
 </file>
@@ -284,7 +296,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -357,6 +369,22 @@
     <font>
       <b/>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="CorpoS"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -467,26 +495,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -537,6 +547,36 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -915,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E12"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -927,175 +967,192 @@
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="7">
         <v>42797</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="135">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="7">
         <v>42801</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="135">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="7">
         <v>42802</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="24" customHeight="1">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="7">
         <v>42802</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="7">
         <v>42802</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="7">
         <v>42803</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.5">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="7">
         <v>42804</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:5" ht="38.25">
+      <c r="A12" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="29">
+        <v>42805</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="17" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="114.75">
+      <c r="A13" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="13">
-        <v>42805</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>74</v>
+      <c r="B13" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="7">
+        <v>42807</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1111,451 +1168,451 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="21" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" style="21" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="21" style="19" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="19" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="19" customWidth="1"/>
-    <col min="11" max="11" width="75.85546875" style="21" customWidth="1"/>
-    <col min="12" max="1025" width="9.140625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="15" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="21" style="13" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="13" customWidth="1"/>
+    <col min="11" max="11" width="75.85546875" style="15" customWidth="1"/>
+    <col min="12" max="1025" width="9.140625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="24" customFormat="1" ht="12.75">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="23" t="s">
+    <row r="3" spans="1:11" s="18" customFormat="1" ht="12.75">
+      <c r="A3" s="23"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="19">
+      <c r="A4" s="13">
         <v>0</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="15">
         <v>0</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="15">
         <v>1</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="19" t="s">
+      <c r="G4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="24" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="19">
+      <c r="A5" s="13">
         <v>1</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="15">
         <v>0</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="15">
         <v>1</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="19" t="s">
+      <c r="G5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" s="24" customFormat="1" ht="11.25">
-      <c r="A6" s="19">
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" s="18" customFormat="1" ht="11.25">
+      <c r="A6" s="13">
         <v>2</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="20">
         <v>0</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="20">
         <v>360</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="20">
         <v>1</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="19" t="s">
+      <c r="G6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" ht="45.75">
-      <c r="A7" s="19">
+      <c r="A7" s="13">
         <v>3</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="27" t="s">
+      <c r="C7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="26"/>
-    </row>
-    <row r="8" spans="1:11" ht="23.25">
-      <c r="A8" s="19">
+      <c r="K7" s="20"/>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A8" s="13">
         <v>4</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="15">
         <v>0</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="15">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="15">
         <v>1</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="19" t="s">
+      <c r="G8" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A9" s="13">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="15">
+        <v>0</v>
+      </c>
+      <c r="D9" s="15">
+        <v>100</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="31.5" customHeight="1">
+      <c r="A10" s="13">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="15">
+        <v>-720</v>
+      </c>
+      <c r="D10" s="15">
+        <v>720</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="23.25">
-      <c r="A9" s="19">
-        <v>5</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="21">
+    <row r="11" spans="1:11" ht="51.75" customHeight="1">
+      <c r="A11" s="13">
+        <v>7</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="13">
+        <v>8</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="15">
         <v>0</v>
       </c>
-      <c r="D9" s="21">
-        <v>100</v>
-      </c>
-      <c r="E9" s="21">
+      <c r="D12" s="15">
+        <v>120</v>
+      </c>
+      <c r="E12" s="15">
         <v>1</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="19" t="s">
+      <c r="F12" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0</v>
+      </c>
+      <c r="D13" s="15">
+        <v>9000</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A14" s="13">
+        <v>10</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I14" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J14" s="21" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="23.25">
-      <c r="A10" s="19">
-        <v>6</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="21">
-        <v>-720</v>
-      </c>
-      <c r="D10" s="21">
-        <v>720</v>
-      </c>
-      <c r="E10" s="21">
-        <v>1</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45.75">
-      <c r="A11" s="19">
-        <v>7</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="19">
-        <v>8</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="21">
-        <v>0</v>
-      </c>
-      <c r="D12" s="21">
-        <v>120</v>
-      </c>
-      <c r="E12" s="21">
-        <v>1</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="19">
-        <v>9</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="21">
-        <v>0</v>
-      </c>
-      <c r="D13" s="21">
-        <v>9000</v>
-      </c>
-      <c r="E13" s="21">
-        <v>1</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="K13" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="23.25">
-      <c r="A14" s="19">
-        <v>10</v>
-      </c>
-      <c r="B14" s="20" t="s">
+      <c r="K14" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="K14" s="21" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed communication matrix for Camera and also fixed the UNIDEB_76 req based on the new signal ids trello card: https://trello.com/c/kTtHCovv/7-rd-camera
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="94">
   <si>
     <t>Change history</t>
   </si>
@@ -364,6 +364,13 @@
 Car position on the X axis,
 Car position on the y axis,
 Car angle
+</t>
+  </si>
+  <si>
+    <t>V2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed Camera signals by adding own lat-lon ego for the Camera
 </t>
   </si>
 </sst>
@@ -636,24 +643,6 @@
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -733,6 +722,24 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1160,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E15"/>
+  <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1177,220 +1184,237 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="7">
         <v>42797</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="135">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="7">
         <v>42801</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="135">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="7">
         <v>42802</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="24" customHeight="1">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="7">
         <v>42802</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="7">
         <v>42802</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="7">
         <v>42803</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.5">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="7">
         <v>42804</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.5">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="15">
         <v>42805</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="114.75">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="7">
         <v>42807</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="104.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="20">
         <v>42816</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="128.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="20">
         <v>42823</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="42.75">
+      <c r="A16" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="20">
+        <v>42825</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1405,630 +1429,697 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK20"/>
+  <dimension ref="A1:AMK22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="30" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="28" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="21" style="28" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="28" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="75.85546875" style="30" customWidth="1"/>
-    <col min="12" max="1025" width="9.140625" style="30" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="24" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="21" style="22" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="75.85546875" style="24" customWidth="1"/>
+    <col min="12" max="1025" width="9.140625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="12.75">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="32" t="s">
+    <row r="3" spans="1:11" s="27" customFormat="1" ht="12.75">
+      <c r="A3" s="32"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="23.25">
-      <c r="A4" s="28">
+      <c r="A4" s="22">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="24">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="24">
         <v>1</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="28" t="s">
+      <c r="G4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="33" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="23.25">
-      <c r="A5" s="28">
+      <c r="A5" s="22">
         <v>1</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="24">
         <v>0</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="24">
         <v>1</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="28" t="s">
+      <c r="G5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="22.5">
-      <c r="A6" s="28">
+      <c r="K5" s="33"/>
+    </row>
+    <row r="6" spans="1:11" s="27" customFormat="1" ht="22.5">
+      <c r="A6" s="22">
         <v>2</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="28">
         <v>0</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="28">
         <v>360</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="28">
         <v>1</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="28" t="s">
+      <c r="G6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" ht="45.75">
-      <c r="A7" s="28">
+      <c r="A7" s="22">
         <v>3</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="35" t="s">
+      <c r="C7" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="34"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A8" s="28">
+      <c r="A8" s="22">
         <v>4</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="24">
         <v>0</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="24">
         <v>1</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="28" t="s">
+      <c r="G8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="29" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A9" s="28">
+      <c r="A9" s="22">
         <v>5</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="24">
         <v>0</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="24">
         <v>100</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="24">
         <v>1</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="28" t="s">
+      <c r="G9" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="29" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5" customHeight="1">
-      <c r="A10" s="28">
+      <c r="A10" s="22">
         <v>6</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="24">
         <v>-720</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="24">
         <v>720</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="24">
         <v>1</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="28" t="s">
+      <c r="G10" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="29" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A11" s="28">
+      <c r="A11" s="22">
         <v>7</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="35" t="s">
+      <c r="C11" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="J11" s="35" t="s">
+      <c r="J11" s="29" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="28">
+      <c r="A12" s="22">
         <v>8</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="24">
         <v>0</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="24">
         <v>120</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="24">
         <v>1</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="28" t="s">
+      <c r="G12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="30" t="s">
+      <c r="K12" s="24" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="28">
+      <c r="A13" s="22">
         <v>9</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="24">
         <v>0</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="24">
         <v>9000</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="24">
         <v>1</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="28" t="s">
+      <c r="G13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="35" t="s">
+      <c r="J13" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="K13" s="30" t="s">
+      <c r="K13" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A14" s="28">
+      <c r="A14" s="22">
         <v>10</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="35" t="s">
+      <c r="C14" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="35" t="s">
+      <c r="J14" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="30" t="s">
+      <c r="K14" s="24" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="28">
+      <c r="A15" s="22">
         <v>11</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="24">
         <v>0</v>
       </c>
-      <c r="D15" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="30">
+      <c r="D15" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="24">
         <v>1</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="28" t="s">
+      <c r="G15" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="28">
+      <c r="A16" s="22">
         <v>12</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="24">
         <v>0</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="30">
+      <c r="D16" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="24">
         <v>1</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="G16" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="28" t="s">
+      <c r="G16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="28">
+      <c r="A17" s="22">
         <v>13</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="24">
         <v>0</v>
       </c>
-      <c r="D17" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="30">
+      <c r="D17" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="28" t="s">
+      <c r="G17" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="28">
+      <c r="A18" s="22">
         <v>14</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="24">
         <v>0</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="30">
+      <c r="D18" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="24">
         <v>1</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="28" t="s">
+      <c r="G18" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="28">
+      <c r="A19" s="22">
         <v>15</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="24">
         <v>0</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="30">
+      <c r="D19" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="24">
         <v>1</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" s="28" t="s">
+      <c r="G19" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="J19" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="28">
+      <c r="A20" s="22">
         <v>16</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I20" s="22" t="s">
         <v>86</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="22">
+        <v>17</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="24">
+        <v>0</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="24">
+        <v>1</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="22">
+        <v>18</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="24">
+        <v>0</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="24">
+        <v>1</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the "filterOut_LessDangerousObjects" method. https://trello.com/c/1FPKdp56
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="88">
   <si>
     <t xml:space="preserve">Change history</t>
   </si>
@@ -173,6 +173,36 @@
     <t xml:space="preserve">Szőke György</t>
   </si>
   <si>
+    <t xml:space="preserve">V1.10</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CorpoS"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Changed signals unit for the Radar Sensor:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">- Longitudinal RVX
+- Longitudinal EGO
+- Lateral RVY
+- Lateral EGO
+</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Communication matrix for the UniDebAutomatedCar project</t>
   </si>
   <si>
@@ -326,9 +356,6 @@
   </si>
   <si>
     <t xml:space="preserve">Longitudinal EGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
   </si>
   <si>
     <t xml:space="preserve">Lateral RVY</t>
@@ -361,16 +388,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -1001,10 +1031,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E14"/>
+  <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1012,7 +1042,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
@@ -1201,7 +1231,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="73.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
         <v>31</v>
       </c>
@@ -1215,6 +1245,23 @@
         <v>42816</v>
       </c>
       <c r="E14" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="65.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="21" t="n">
+        <v>42828</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1240,27 +1287,27 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="25" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="23" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="25" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="23" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="23" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="23" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="23" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="23" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="23" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="75.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="25" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="25" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1274,54 +1321,54 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
       <c r="G2" s="27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27"/>
       <c r="B3" s="28"/>
       <c r="C3" s="30" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,34 +1376,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" s="25" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,31 +1411,31 @@
         <v>1</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C5" s="25" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E5" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K5" s="33"/>
     </row>
@@ -1397,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C6" s="34" t="n">
         <v>0</v>
@@ -1409,19 +1456,19 @@
         <v>1</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K6" s="33"/>
     </row>
@@ -1430,29 +1477,29 @@
         <v>3</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E7" s="34"/>
       <c r="F7" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J7" s="35" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K7" s="34"/>
     </row>
@@ -1461,7 +1508,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C8" s="25" t="n">
         <v>0</v>
@@ -1473,19 +1520,19 @@
         <v>1</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J8" s="35" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1493,7 +1540,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C9" s="25" t="n">
         <v>0</v>
@@ -1505,19 +1552,19 @@
         <v>1</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J9" s="35" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1525,7 +1572,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10" s="25" t="n">
         <v>-720</v>
@@ -1537,19 +1584,19 @@
         <v>1</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J10" s="35" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1557,28 +1604,28 @@
         <v>7</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J11" s="35" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,7 +1633,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C12" s="25" t="n">
         <v>0</v>
@@ -1598,22 +1645,22 @@
         <v>1</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,7 +1668,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C13" s="25" t="n">
         <v>0</v>
@@ -1633,22 +1680,22 @@
         <v>1</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K13" s="25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1656,34 +1703,34 @@
         <v>10</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J14" s="35" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,31 +1738,31 @@
         <v>11</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C15" s="25" t="n">
         <v>0</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E15" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1723,31 +1770,31 @@
         <v>12</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C16" s="25" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E16" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>81</v>
-      </c>
       <c r="J16" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,31 +1802,31 @@
         <v>13</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C17" s="25" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E17" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H17" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,31 +1834,31 @@
         <v>14</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="25" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E18" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>81</v>
-      </c>
       <c r="J18" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,31 +1866,31 @@
         <v>15</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C19" s="25" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E19" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed documents (commmatrix, requirements).
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Version &amp; History" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="CommunicationMatrix" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="explanatory pictures" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">CommunicationMatrix!$A$2:$J$10</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="97">
   <si>
     <t xml:space="preserve">Change history</t>
   </si>
@@ -173,34 +174,36 @@
     <t xml:space="preserve">Szőke György</t>
   </si>
   <si>
-    <t xml:space="preserve">V1.10</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="CorpoS"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Changed signals unit for the Radar Sensor:
+    <t xml:space="preserve">V2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Traffic sign meaning signal for the Camera module:
+Added new worksheet with explanatory picture of the traffic sign values
+Added Camera module as a receiver of these signals:
+Car position on the X axis,
+Car position on the y axis,
+Car angle
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">- Longitudinal RVX
+  </si>
+  <si>
+    <t xml:space="preserve">V2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed Camera signals by adding own lat-lon ego for the Camera
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed signals unit for the Radar Sensor:
+- Longitudinal RVX
 - Longitudinal EGO
 - Lateral RVY
-- Lateral EGO
-</t>
-    </r>
+- Lateral EGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04.03.2017</t>
   </si>
   <si>
     <t xml:space="preserve">Communication matrix for the UniDebAutomatedCar project</t>
@@ -263,7 +266,8 @@
     <t xml:space="preserve">PowertrainSystem</t>
   </si>
   <si>
-    <t xml:space="preserve">AutomatedCar</t>
+    <t xml:space="preserve">AutomatedCar
+Camera</t>
   </si>
   <si>
     <t xml:space="preserve">These signals go directly to the AutomatedCar</t>
@@ -358,6 +362,9 @@
     <t xml:space="preserve">Longitudinal EGO</t>
   </si>
   <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lateral RVY</t>
   </si>
   <si>
@@ -365,6 +372,15 @@
   </si>
   <si>
     <t xml:space="preserve">Object Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic sign meaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can be seen on the next worksheet "explanatory pictures"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera</t>
   </si>
 </sst>
 </file>
@@ -388,19 +404,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -793,7 +806,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -886,6 +899,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -922,8 +939,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1026,15 +1043,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>549360</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>29520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Kép 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5400720" cy="4791960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E15"/>
+  <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1042,7 +1101,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
@@ -1112,7 +1171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="85.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -1197,7 +1256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -1214,7 +1273,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
@@ -1231,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="104.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
         <v>31</v>
       </c>
@@ -1248,7 +1307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="65.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="128.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
         <v>34</v>
       </c>
@@ -1256,15 +1315,53 @@
         <v>35</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D15" s="21" t="n">
-        <v>42828</v>
+        <v>42823</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="21" t="n">
+        <v>42825</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="60.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:D2"/>
@@ -1284,613 +1381,697 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="25" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="23" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="23" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="23" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="23" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="75.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="25" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="26" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="24" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="24" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="24" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="24" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="75.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="26" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="A1" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="C2" s="30" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="30" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="H2" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="I2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="J2" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="n">
+    <row r="3" s="32" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="25" t="n">
+      <c r="B4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="25" t="n">
+      <c r="D4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="32" t="s">
+      <c r="F4" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="E5" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="n">
+      <c r="G5" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="34"/>
+    </row>
+    <row r="6" s="32" customFormat="true" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="35" t="n">
+        <v>360</v>
+      </c>
+      <c r="E6" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="25" t="n">
+      <c r="F6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="34"/>
+    </row>
+    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="35"/>
+      <c r="F7" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="35"/>
+    </row>
+    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="25" t="n">
+      <c r="D8" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="33"/>
-    </row>
-    <row r="6" s="31" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="24" t="s">
+      <c r="F8" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="24" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="24" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="26" t="n">
+        <v>-720</v>
+      </c>
+      <c r="D10" s="26" t="n">
+        <v>720</v>
+      </c>
+      <c r="E10" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="24" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="24" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="26" t="n">
+        <v>120</v>
+      </c>
+      <c r="E12" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="34" t="n">
+      <c r="I12" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="24" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="34" t="n">
-        <v>360</v>
-      </c>
-      <c r="E6" s="34" t="n">
+      <c r="D13" s="26" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E13" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F13" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="33"/>
-    </row>
-    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="34"/>
-    </row>
-    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="25" t="n">
+      <c r="J13" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="24" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="25" t="n">
-        <v>100</v>
-      </c>
-      <c r="E8" s="25" t="n">
+      <c r="D15" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="25" t="n">
+      <c r="F15" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="24" t="n">
+        <v>12</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="25" t="n">
-        <v>100</v>
-      </c>
-      <c r="E9" s="25" t="n">
+      <c r="D16" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="25" t="n">
-        <v>-720</v>
-      </c>
-      <c r="D10" s="25" t="n">
-        <v>720</v>
-      </c>
-      <c r="E10" s="25" t="n">
+      <c r="F16" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="24" t="n">
+        <v>13</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F17" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="25" t="n">
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="24" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="25" t="n">
-        <v>120</v>
-      </c>
-      <c r="E12" s="25" t="n">
+      <c r="D18" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="25" t="n">
+      <c r="F18" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="24" t="n">
+        <v>15</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="25" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E13" s="25" t="n">
+      <c r="D19" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="K14" s="25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23" t="n">
-        <v>11</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="25" t="n">
+      <c r="F19" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="24" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="24" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="25" t="n">
+      <c r="D21" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="n">
-        <v>12</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="25" t="n">
+      <c r="F21" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="24" t="n">
+        <v>18</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="25" t="n">
+      <c r="D22" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23" t="n">
-        <v>13</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="n">
-        <v>14</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23" t="n">
-        <v>15</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>55</v>
+      <c r="F22" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1914,4 +2095,31 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.6"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Signal 11,12,13,14,15 unit
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version &amp; History" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="98">
   <si>
     <t xml:space="preserve">Change history</t>
   </si>
@@ -356,31 +356,34 @@
     <t xml:space="preserve">Longitudinal RVX</t>
   </si>
   <si>
+    <t xml:space="preserve">pixel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Radar Sensor</t>
   </si>
   <si>
     <t xml:space="preserve">Longitudinal EGO</t>
   </si>
   <si>
+    <t xml:space="preserve">Lateral RVY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lateral EGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic sign meaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can be seen on the next worksheet "explanatory pictures"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera</t>
+  </si>
+  <si>
     <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral RVY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral EGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traffic sign meaning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can be seen on the next worksheet "explanatory pictures"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camera</t>
   </si>
 </sst>
 </file>
@@ -1054,9 +1057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>549360</xdr:colOff>
+      <xdr:colOff>549000</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1070,7 +1073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5400720" cy="4791960"/>
+          <a:ext cx="5405400" cy="4791600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1092,7 +1095,7 @@
   </sheetPr>
   <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -1101,7 +1104,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
@@ -1383,23 +1386,23 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="26" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="24" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="24" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="24" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="26" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="24" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="24" width="21.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="24" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="24" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="24" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="75.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="26" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="26" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="G15" s="24" t="s">
         <v>58</v>
@@ -1856,18 +1859,18 @@
         <v>59</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J15" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="n">
         <v>12</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" s="26" t="n">
         <v>0</v>
@@ -1879,7 +1882,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G16" s="24" t="s">
         <v>58</v>
@@ -1888,13 +1891,13 @@
         <v>59</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J16" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="n">
         <v>13</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="G17" s="24" t="s">
         <v>58</v>
@@ -1920,13 +1923,13 @@
         <v>59</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J17" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="n">
         <v>14</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>58</v>
@@ -1952,7 +1955,7 @@
         <v>59</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J18" s="24" t="s">
         <v>60</v>
@@ -1975,7 +1978,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="G19" s="24" t="s">
         <v>58</v>
@@ -1984,7 +1987,7 @@
         <v>59</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J19" s="24" t="s">
         <v>60</v>
@@ -2027,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>58</v>
@@ -2047,7 +2050,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C22" s="26" t="n">
         <v>0</v>
@@ -2059,7 +2062,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="G22" s="24" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Changed the way the radar sensor communicates
with the car as pointed out by team2. Now the communication is trough
the VirtualFunctionBus.

Further changes like this are coming up.
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="104">
   <si>
     <t xml:space="preserve">Change history</t>
   </si>
@@ -206,6 +206,36 @@
     <t xml:space="preserve">04.03.2017</t>
   </si>
   <si>
+    <t xml:space="preserve">V2.3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Added:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">Radar Sensor PosX
+Radar Sensor PosY</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">04.11.2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">Communication matrix for the UniDebAutomatedCar project</t>
   </si>
   <si>
@@ -384,6 +414,15 @@
   </si>
   <si>
     <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radar Sensor PosX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutomatedCar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radar Sensor PosY</t>
   </si>
 </sst>
 </file>
@@ -395,7 +434,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YYYY"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -551,6 +590,13 @@
       <name val="CorpoS"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="8"/>
@@ -635,7 +681,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -694,6 +740,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
       <top/>
@@ -809,7 +862,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -906,55 +959,67 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1057,9 +1122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>549000</xdr:colOff>
+      <xdr:colOff>548640</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1073,7 +1138,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5405400" cy="4791600"/>
+          <a:ext cx="5405040" cy="4791240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1093,10 +1158,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E18"/>
+  <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1361,7 +1426,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="34.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1384,697 +1465,761 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="26" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="24" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="24" width="21.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="24" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="24" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="24" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="75.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="26" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="29" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="27" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="21.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="27" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="27" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="29" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="29" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="A1" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="28" t="s">
+      <c r="A2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="C2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="H2" s="31" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" s="32" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="31" t="s">
+      <c r="I2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="J2" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="K2" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="28" t="s">
+    </row>
+    <row r="3" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28" t="s">
+      <c r="D3" s="34" t="s">
         <v>54</v>
       </c>
+      <c r="E3" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="n">
+      <c r="A4" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="26" t="n">
+      <c r="B4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="26" t="n">
+      <c r="D4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="24" t="s">
+      <c r="F4" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="E5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" s="34" t="s">
+      <c r="G5" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="n">
+      <c r="I5" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="37"/>
+    </row>
+    <row r="6" s="35" customFormat="true" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="38" t="n">
+        <v>360</v>
+      </c>
+      <c r="E6" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="F6" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="26" t="n">
+      <c r="J6" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="37"/>
+    </row>
+    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="38"/>
+    </row>
+    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="26" t="n">
+      <c r="D8" s="29" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="24" t="s">
+      <c r="F8" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="29" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="29" t="n">
+        <v>-720</v>
+      </c>
+      <c r="D10" s="29" t="n">
+        <v>720</v>
+      </c>
+      <c r="E10" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="27" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="27" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29" t="n">
+        <v>120</v>
+      </c>
+      <c r="E12" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="27" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="29" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E13" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="27" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="27" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="27" t="n">
+        <v>12</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="27" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="27" t="n">
+        <v>15</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="27" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="27" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="27" t="n">
+        <v>18</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="27" t="n">
+        <v>19</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="34"/>
-    </row>
-    <row r="6" s="32" customFormat="true" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="35" t="n">
+      <c r="E23" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="27" t="n">
+        <v>20</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="35" t="n">
-        <v>360</v>
-      </c>
-      <c r="E6" s="35" t="n">
+      <c r="D24" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" s="34"/>
-    </row>
-    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" s="35"/>
-    </row>
-    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="26" t="n">
-        <v>100</v>
-      </c>
-      <c r="E8" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="26" t="n">
-        <v>100</v>
-      </c>
-      <c r="E9" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="26" t="n">
-        <v>-720</v>
-      </c>
-      <c r="D10" s="26" t="n">
-        <v>720</v>
-      </c>
-      <c r="E10" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J11" s="36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="26" t="n">
-        <v>120</v>
-      </c>
-      <c r="E12" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="26" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E13" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="J13" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J14" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" s="26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="n">
-        <v>11</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="n">
-        <v>12</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="n">
-        <v>13</v>
-      </c>
-      <c r="B17" s="25" t="s">
+      <c r="F24" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="n">
-        <v>14</v>
-      </c>
-      <c r="B18" s="25" t="s">
+      <c r="G24" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" s="27" t="s">
         <v>92</v>
-      </c>
-      <c r="C18" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="n">
-        <v>15</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="n">
-        <v>16</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="n">
-        <v>17</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="n">
-        <v>18</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed signals in commatrix and in the code.
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="108">
   <si>
     <t xml:space="preserve">Change history</t>
   </si>
@@ -236,6 +236,36 @@
     <t xml:space="preserve">04.11.2017</t>
   </si>
   <si>
+    <t xml:space="preserve">V2.4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Changed:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">Longitudinal RVX → Radar Longitudinal Relative Velocity
+Longitudinal EGO → Radar Longitudinal Distance From EGO
+Lateral RVY → Radar Lateral Relative Velocity
+Lateral EGO → Radar Lateral Distance From EGO
+</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Communication matrix for the UniDebAutomatedCar project</t>
   </si>
   <si>
@@ -383,7 +413,7 @@
     <t xml:space="preserve">This signal will set the visual indicator for the headlight state</t>
   </si>
   <si>
-    <t xml:space="preserve">Longitudinal RVX</t>
+    <t xml:space="preserve">Radar Longitudinal Relative Velocity</t>
   </si>
   <si>
     <t xml:space="preserve">pixel</t>
@@ -392,28 +422,34 @@
     <t xml:space="preserve">Radar Sensor</t>
   </si>
   <si>
+    <t xml:space="preserve">Radar Longitudinal Distance From EGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radar Lateral Relative Velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radar Lateral Distance From EGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic sign meaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can be seen on the next worksheet "explanatory pictures"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lateral EGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
     <t xml:space="preserve">Longitudinal EGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral RVY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral EGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traffic sign meaning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can be seen on the next worksheet "explanatory pictures"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
   </si>
   <si>
     <t xml:space="preserve">Radar Sensor PosX</t>
@@ -446,16 +482,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -1122,9 +1161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
+      <xdr:colOff>548280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1138,7 +1177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5405040" cy="4791240"/>
+          <a:ext cx="5404680" cy="4790880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1158,10 +1197,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E19"/>
+  <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1443,7 +1482,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="83.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1467,14 +1522,14 @@
   </sheetPr>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="24.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="29" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="27" width="9.13"/>
@@ -1488,7 +1543,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1502,54 +1557,54 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K2" s="31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="C3" s="34" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
       <c r="K3" s="31" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1557,34 +1612,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C4" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E4" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,31 +1647,31 @@
         <v>1</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C5" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E5" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K5" s="37"/>
     </row>
@@ -1625,7 +1680,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C6" s="38" t="n">
         <v>0</v>
@@ -1637,19 +1692,19 @@
         <v>1</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K6" s="37"/>
     </row>
@@ -1658,29 +1713,29 @@
         <v>3</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K7" s="38"/>
     </row>
@@ -1689,7 +1744,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C8" s="29" t="n">
         <v>0</v>
@@ -1701,19 +1756,19 @@
         <v>1</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1721,7 +1776,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C9" s="29" t="n">
         <v>0</v>
@@ -1733,19 +1788,19 @@
         <v>1</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1753,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C10" s="29" t="n">
         <v>-720</v>
@@ -1765,19 +1820,19 @@
         <v>1</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1785,28 +1840,28 @@
         <v>7</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,7 +1869,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C12" s="29" t="n">
         <v>0</v>
@@ -1826,22 +1881,22 @@
         <v>1</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1849,7 +1904,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C13" s="29" t="n">
         <v>0</v>
@@ -1861,22 +1916,22 @@
         <v>1</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H13" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K13" s="29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1884,66 +1939,66 @@
         <v>10</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G14" s="39" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J14" s="39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K14" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="n">
         <v>11</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C15" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E15" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,31 +2006,31 @@
         <v>12</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C16" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E16" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1983,31 +2038,31 @@
         <v>13</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C17" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E17" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,31 +2070,31 @@
         <v>14</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C18" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E18" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,31 +2102,31 @@
         <v>15</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C19" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E19" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,19 +2134,19 @@
         <v>16</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2099,31 +2154,31 @@
         <v>17</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C21" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E21" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,31 +2186,31 @@
         <v>18</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C22" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E22" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,31 +2218,31 @@
         <v>19</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C23" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E23" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2195,31 +2250,31 @@
         <v>20</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C24" s="29" t="n">
         <v>0</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E24" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the commMatrix with TSR signals
https://trello.com/c/rfd39KBc
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Version &amp; History" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="116">
   <si>
     <t xml:space="preserve">Change history</t>
   </si>
@@ -266,6 +266,32 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">V2.5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Added:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">MOST RELEVANT SPEED LIMIT
+SHOW SUPPLEMENTAL SIGNS ON IC</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Communication matrix for the UniDebAutomatedCar project</t>
   </si>
   <si>
@@ -459,6 +485,27 @@
   </si>
   <si>
     <t xml:space="preserve">Radar Sensor PosY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOST RELEVANT SPEED LIMIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, ACC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHOW SUPPLEMENTAL SIGNS ON IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Speed Limit: 0
+STOP: 1
+In City Speed Limit 60: 2
+Yield!: 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC</t>
   </si>
 </sst>
 </file>
@@ -470,7 +517,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YYYY"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -482,19 +529,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -636,6 +680,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -901,7 +951,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1010,56 +1060,64 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1161,9 +1219,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>548280</xdr:colOff>
+      <xdr:colOff>547920</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1177,7 +1235,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5404680" cy="4790880"/>
+          <a:ext cx="5404320" cy="4790520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1199,8 +1257,8 @@
   </sheetPr>
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1499,8 +1557,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="34.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:D2"/>
@@ -1520,763 +1593,837 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="24.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="29" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="27" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="21.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="27" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="27" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="29" width="75.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="29" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="24.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="30" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="28" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="28" width="21.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="28" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="28" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="28" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="30" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="30" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="A1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="31" t="s">
+      <c r="B2" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="C2" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="H2" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="I2" s="32" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="34" t="s">
+      <c r="J2" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="K2" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="34" t="s">
+    </row>
+    <row r="3" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="D3" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31" t="s">
+      <c r="E3" s="35" t="s">
         <v>59</v>
       </c>
+      <c r="F3" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="n">
+      <c r="A4" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="29" t="n">
+      <c r="B4" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="29" t="n">
+      <c r="D4" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="27" t="s">
+      <c r="F4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="E5" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="36" t="s">
+      <c r="G5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="I5" s="28" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="n">
+      <c r="J5" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" s="36" customFormat="true" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="39" t="n">
+        <v>360</v>
+      </c>
+      <c r="E6" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="F6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="29" t="n">
+      <c r="K6" s="38"/>
+    </row>
+    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="39"/>
+      <c r="F7" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="39"/>
+    </row>
+    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="29" t="n">
+      <c r="D8" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="27" t="s">
+      <c r="F8" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="30" t="n">
+        <v>-720</v>
+      </c>
+      <c r="D10" s="30" t="n">
+        <v>720</v>
+      </c>
+      <c r="E10" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="28" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="28" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="30" t="n">
+        <v>120</v>
+      </c>
+      <c r="E12" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="28" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="30" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E13" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="28" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28" t="n">
+        <v>12</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28" t="n">
+        <v>15</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="28" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="28" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="28" t="n">
+        <v>18</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="28" t="n">
+        <v>19</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="36" t="s">
+      <c r="E23" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="37"/>
-    </row>
-    <row r="6" s="35" customFormat="true" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="38" t="n">
+      <c r="I23" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="38" t="n">
-        <v>360</v>
-      </c>
-      <c r="E6" s="38" t="n">
+      <c r="D24" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" s="36" t="s">
+      <c r="F24" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="37"/>
-    </row>
-    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J7" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="K7" s="38"/>
-    </row>
-    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="29" t="n">
-        <v>100</v>
-      </c>
-      <c r="E8" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="n">
+      <c r="I24" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28" t="n">
+        <v>21</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="30" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="29" t="n">
-        <v>100</v>
-      </c>
-      <c r="E9" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="29" t="n">
-        <v>-720</v>
-      </c>
-      <c r="D10" s="29" t="n">
-        <v>720</v>
-      </c>
-      <c r="E10" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="29" t="n">
-        <v>120</v>
-      </c>
-      <c r="E12" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="29" t="s">
+      <c r="D25" s="30" t="n">
+        <v>130</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="28" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="29" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E13" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="K14" s="29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="n">
-        <v>11</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="J15" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27" t="n">
-        <v>12</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="n">
-        <v>13</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27" t="n">
-        <v>14</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27" t="n">
-        <v>15</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="J19" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27" t="n">
-        <v>16</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="J20" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="27" t="n">
-        <v>17</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="J21" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="n">
-        <v>18</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="G22" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="J22" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27" t="n">
-        <v>19</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27" t="n">
-        <v>20</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I24" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="J24" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
+      <c r="G25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="28" t="n">
+        <v>22</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:J1"/>

</xml_diff>

<commit_message>
Updated commMatrix for upcoming change to PT to IC communication.
Added new signal IDs to signalDatabase.
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version &amp; History" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="121">
   <si>
     <t xml:space="preserve">Change history</t>
   </si>
@@ -275,6 +275,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Added:
 </t>
@@ -292,6 +293,63 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">V2.6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Added:
+POWERTRAIN STEERING WHEEL ANGLE
+POWERTRAIN GEAR POSITION
+POWERTRAIN HEADLIGHT
+POWERTRAIN INDEX INDICATORS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Updated signal id: 0
+Updated signal id: 1
+Updated signal id: 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Updated signal id: 3
+Updated signal id: 6
+Updated signal id: 7
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Updated signal id: 10</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">04.12.2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">Communication matrix for the UniDebAutomatedCar project</t>
   </si>
   <si>
@@ -353,7 +411,8 @@
   </si>
   <si>
     <t xml:space="preserve">AutomatedCar
-Camera</t>
+Camera
+RadarSensor</t>
   </si>
   <si>
     <t xml:space="preserve">These signals go directly to the AutomatedCar</t>
@@ -383,10 +442,6 @@
     <t xml:space="preserve">HMI</t>
   </si>
   <si>
-    <t xml:space="preserve">PowertrainSystem
-Instrument Cluster</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gas pedal position</t>
   </si>
   <si>
@@ -436,9 +491,6 @@
 OFF: 0</t>
   </si>
   <si>
-    <t xml:space="preserve">This signal will set the visual indicator for the headlight state</t>
-  </si>
-  <si>
     <t xml:space="preserve">Radar Longitudinal Relative Velocity</t>
   </si>
   <si>
@@ -506,6 +558,18 @@
   </si>
   <si>
     <t xml:space="preserve">IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POWERTRAIN STEERING WHEEL ANGLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POWERTRAIN GEAR POSITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POWERTRAIN HEADLIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POWERTRAIN INDEX INDICATORS</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1124,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1110,6 +1170,10 @@
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1219,9 +1283,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>547920</xdr:colOff>
+      <xdr:colOff>547560</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1235,7 +1299,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5404320" cy="4790520"/>
+          <a:ext cx="5403960" cy="4790160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1255,10 +1319,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E20"/>
+  <dimension ref="A2:E21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1561,7 +1625,7 @@
       <c r="A20" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="25" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="26" t="s">
@@ -1571,6 +1635,23 @@
         <v>43</v>
       </c>
       <c r="E20" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="128.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1593,831 +1674,952 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="24.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="30" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="28" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="28" width="21.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="28" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="28" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="28" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="30" width="75.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="30" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="25.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="29" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="27" width="4.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="21.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="27" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="27" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="29" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="29" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="A1" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="B2" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="35" t="s">
+      <c r="I2" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="J2" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="K2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="32" t="s">
+    </row>
+    <row r="3" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32" t="s">
+      <c r="D3" s="34" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="n">
+      <c r="E3" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="25.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="30" t="n">
+      <c r="B4" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="30" t="n">
+      <c r="D4" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="28" t="s">
+      <c r="F4" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="25.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="E5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="38" t="s">
+      <c r="G5" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28" t="n">
+      <c r="I5" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="37"/>
+    </row>
+    <row r="6" s="35" customFormat="true" ht="25.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="38" t="n">
+        <v>360</v>
+      </c>
+      <c r="E6" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="F6" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="30" t="n">
+      <c r="J6" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="37"/>
+    </row>
+    <row r="7" customFormat="false" ht="32.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="38"/>
+    </row>
+    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="30" t="n">
+      <c r="D8" s="29" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="28" t="s">
+      <c r="F8" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="29" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="29" t="n">
+        <v>-720</v>
+      </c>
+      <c r="D10" s="29" t="n">
+        <v>720</v>
+      </c>
+      <c r="E10" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="27" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="27" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29" t="n">
+        <v>120</v>
+      </c>
+      <c r="E12" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="27" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="29" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E13" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="27" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="27" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="27" t="n">
+        <v>12</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="27" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="27" t="n">
+        <v>15</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="27" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="27" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="27" t="n">
+        <v>18</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="27" t="n">
+        <v>19</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="38"/>
-    </row>
-    <row r="6" s="36" customFormat="true" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="39" t="n">
+      <c r="E23" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="27" t="n">
+        <v>20</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="39" t="n">
-        <v>360</v>
-      </c>
-      <c r="E6" s="39" t="n">
+      <c r="D24" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="38"/>
-    </row>
-    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="28" t="s">
+      <c r="F24" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="27" t="n">
+        <v>21</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="29" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="29" t="n">
+        <v>130</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="32.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="27" t="n">
+        <v>22</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="27" t="n">
+        <v>23</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="29" t="n">
+        <v>-720</v>
+      </c>
+      <c r="D27" s="29" t="n">
+        <v>720</v>
+      </c>
+      <c r="E27" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" s="40" t="s">
+      <c r="G27" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="32.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="27" t="n">
+        <v>24</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J29" s="40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="32.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="39"/>
-    </row>
-    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="30" t="n">
-        <v>100</v>
-      </c>
-      <c r="E8" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="30" t="n">
-        <v>100</v>
-      </c>
-      <c r="E9" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="30" t="n">
-        <v>-720</v>
-      </c>
-      <c r="D10" s="30" t="n">
-        <v>720</v>
-      </c>
-      <c r="E10" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="28" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="30" t="n">
-        <v>120</v>
-      </c>
-      <c r="E12" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="30" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E13" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="H14" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="K14" s="30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J15" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="n">
-        <v>12</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J16" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28" t="n">
-        <v>13</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28" t="n">
-        <v>14</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28" t="n">
-        <v>15</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J19" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28" t="n">
-        <v>16</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="J20" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="n">
-        <v>17</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="n">
-        <v>18</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="J22" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28" t="n">
-        <v>19</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28" t="n">
-        <v>20</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="J24" s="28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28" t="n">
-        <v>21</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="D25" s="30" t="n">
-        <v>130</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="J25" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="n">
-        <v>22</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="J26" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H30" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J30" s="40" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
[RD] ACC - Added some remaining requirement - trello card: https://trello.com/c/WUu8Vk9U/23-rd-acc
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="144">
   <si>
     <t>Change history</t>
   </si>
@@ -609,14 +609,57 @@
     <t>ACC status changed</t>
   </si>
   <si>
-    <t>ACTIVE: 1
-DISABLED: 0</t>
-  </si>
-  <si>
     <t>HMI, ACC</t>
   </si>
   <si>
     <t>ACC, HMI</t>
+  </si>
+  <si>
+    <t>CRUISE CONTROL SPEED: 0
+SAFE DISTANCE: 1</t>
+  </si>
+  <si>
+    <t>ACC setting switched</t>
+  </si>
+  <si>
+    <t>ACC change value</t>
+  </si>
+  <si>
+    <t>V3.0</t>
+  </si>
+  <si>
+    <t>04.26.2017</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ACC setting switched signal (ID 30)
+ACC change value signal (ID 31)
+Extended ACC status changed signal (ID 29) with logical values</t>
+    </r>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>DISABLED: 0
+ACTIVE: 1
+SUSPENDED: 2
+STOPANDGO: 3</t>
+  </si>
+  <si>
+    <t>DECREMENT: 0
+INCREMENT: 1</t>
   </si>
 </sst>
 </file>
@@ -921,24 +964,6 @@
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1039,6 +1064,24 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1459,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E24"/>
+  <dimension ref="A2:E25"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1476,373 +1519,390 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="7">
         <v>42797</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="135">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="7">
         <v>42801</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="135">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="7">
         <v>42802</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="24" customHeight="1">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="7">
         <v>42802</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="7">
         <v>42802</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="7">
         <v>42803</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.5">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="7">
         <v>42804</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.5">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="15">
         <v>42805</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="114.75">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="7">
         <v>42807</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="104.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="20">
         <v>42816</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="128.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="20">
         <v>42823</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="42.75">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="20">
         <v>42825</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="71.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="46.5">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="125.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="46.5">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="180">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="75">
+      <c r="A25" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1857,1043 +1917,1107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK33"/>
+  <dimension ref="A1:AMK35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="34" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" style="32" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="32" customWidth="1"/>
-    <col min="8" max="8" width="21" style="32" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="32" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="32" customWidth="1"/>
-    <col min="11" max="11" width="75.85546875" style="34" customWidth="1"/>
-    <col min="12" max="1025" width="9.140625" style="34" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="28" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="26" customWidth="1"/>
+    <col min="8" max="8" width="21" style="26" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="26" customWidth="1"/>
+    <col min="11" max="11" width="75.85546875" style="28" customWidth="1"/>
+    <col min="12" max="1025" width="9.140625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="37" customFormat="1" ht="12.75">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="36" t="s">
+    <row r="3" spans="1:11" s="31" customFormat="1" ht="12.75">
+      <c r="A3" s="39"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="34.5">
-      <c r="A4" s="32">
+      <c r="A4" s="26">
         <v>0</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="28">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="28">
         <v>1</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="32" t="s">
+      <c r="G4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="40" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="34.5">
-      <c r="A5" s="32">
+      <c r="A5" s="26">
         <v>1</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="28">
         <v>0</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="28">
         <v>1</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" s="32" t="s">
+      <c r="G5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" s="37" customFormat="1" ht="33.75">
-      <c r="A6" s="32">
+      <c r="K5" s="40"/>
+    </row>
+    <row r="6" spans="1:11" s="31" customFormat="1" ht="33.75">
+      <c r="A6" s="26">
         <v>2</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="33">
         <v>0</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="33">
         <v>360</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="33">
         <v>1</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="32" t="s">
+      <c r="G6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="40" t="s">
+      <c r="J6" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" ht="45.75">
-      <c r="A7" s="32">
+      <c r="A7" s="26">
         <v>3</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="41" t="s">
+      <c r="C7" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="33"/>
+      <c r="F7" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="39"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A8" s="32">
+      <c r="A8" s="26">
         <v>4</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="28">
         <v>0</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="28">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="28">
         <v>1</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="32" t="s">
+      <c r="G8" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A9" s="32">
+      <c r="A9" s="26">
         <v>5</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="28">
         <v>0</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="28">
         <v>100</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="28">
         <v>1</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="32" t="s">
+      <c r="G9" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J9" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5" customHeight="1">
-      <c r="A10" s="32">
+      <c r="A10" s="26">
         <v>6</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="28">
         <v>-720</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="28">
         <v>720</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="28">
         <v>1</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="32" t="s">
+      <c r="G10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A11" s="32">
+      <c r="A11" s="26">
         <v>7</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="41" t="s">
+      <c r="C11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J11" s="41" t="s">
+      <c r="J11" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="32">
+      <c r="A12" s="26">
         <v>8</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="28">
         <v>0</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="28">
         <v>120</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="28">
         <v>1</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="32" t="s">
+      <c r="G12" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="32" t="s">
+      <c r="I12" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="41" t="s">
+      <c r="J12" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="28" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="32">
+      <c r="A13" s="26">
         <v>9</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="28">
         <v>0</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="28">
         <v>9000</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="28">
         <v>1</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" s="32" t="s">
+      <c r="G13" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="K13" s="34" t="s">
+      <c r="K13" s="28" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A14" s="32">
+      <c r="A14" s="26">
         <v>10</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="41" t="s">
+      <c r="C14" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I14" s="32" t="s">
+      <c r="I14" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J14" s="41" t="s">
+      <c r="J14" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="32">
+      <c r="A15" s="26">
         <v>11</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="28">
         <v>0</v>
       </c>
-      <c r="D15" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="34">
+      <c r="D15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="28">
         <v>1</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="32" t="s">
+      <c r="G15" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="32" t="s">
+      <c r="I15" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J15" s="32" t="s">
+      <c r="J15" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="32">
+      <c r="A16" s="26">
         <v>12</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="28">
         <v>0</v>
       </c>
-      <c r="D16" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="34">
+      <c r="D16" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="28">
         <v>1</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G16" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="32" t="s">
+      <c r="G16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="32" t="s">
+      <c r="I16" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J16" s="32" t="s">
+      <c r="J16" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="32">
+      <c r="A17" s="26">
         <v>13</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="28">
         <v>0</v>
       </c>
-      <c r="D17" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="34">
+      <c r="D17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="28">
         <v>1</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G17" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="32" t="s">
+      <c r="G17" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I17" s="32" t="s">
+      <c r="I17" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="32" t="s">
+      <c r="J17" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="32">
+      <c r="A18" s="26">
         <v>14</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="28">
         <v>0</v>
       </c>
-      <c r="D18" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="34">
+      <c r="D18" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="28">
         <v>1</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="32" t="s">
+      <c r="G18" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="32">
+      <c r="A19" s="26">
         <v>15</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="28">
         <v>0</v>
       </c>
-      <c r="D19" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="34">
+      <c r="D19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="28">
         <v>1</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="32" t="s">
+      <c r="G19" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="I19" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="32">
+      <c r="A20" s="26">
         <v>16</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I20" s="32" t="s">
+      <c r="I20" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="J20" s="32" t="s">
+      <c r="J20" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="32">
+      <c r="A21" s="26">
         <v>17</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="28">
         <v>0</v>
       </c>
-      <c r="D21" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="34">
+      <c r="D21" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="28">
         <v>1</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G21" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="32" t="s">
+      <c r="G21" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I21" s="32" t="s">
+      <c r="I21" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="J21" s="32" t="s">
+      <c r="J21" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="32">
+      <c r="A22" s="26">
         <v>18</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="28">
         <v>0</v>
       </c>
-      <c r="D22" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="34">
+      <c r="D22" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="28">
         <v>1</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="32" t="s">
+      <c r="G22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="32" t="s">
+      <c r="J22" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="32">
+      <c r="A23" s="26">
         <v>19</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="28">
         <v>0</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="28">
         <v>1</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G23" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" s="32" t="s">
+      <c r="G23" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I23" s="32" t="s">
+      <c r="I23" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="J23" s="32" t="s">
+      <c r="J23" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="32">
+      <c r="A24" s="26">
         <v>20</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="28">
         <v>0</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="28">
         <v>1</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G24" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="32" t="s">
+      <c r="G24" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I24" s="32" t="s">
+      <c r="I24" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="32">
+      <c r="A25" s="26">
         <v>21</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="28">
         <v>5</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="28">
         <v>130</v>
       </c>
-      <c r="E25" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="32" t="s">
+      <c r="E25" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G25" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="32" t="s">
+      <c r="G25" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I25" s="32" t="s">
+      <c r="I25" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="J25" s="32" t="s">
+      <c r="J25" s="26" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="45.75">
-      <c r="A26" s="32">
+      <c r="A26" s="26">
         <v>22</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" s="42" t="s">
+      <c r="C26" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="H26" s="32" t="s">
+      <c r="H26" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I26" s="32" t="s">
+      <c r="I26" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="J26" s="32" t="s">
+      <c r="J26" s="26" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="32">
+      <c r="A27" s="26">
         <v>23</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="34">
+      <c r="C27" s="28">
         <v>-720</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="28">
         <v>720</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="28">
         <v>1</v>
       </c>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" s="32" t="s">
+      <c r="G27" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I27" s="32" t="s">
+      <c r="I27" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J27" s="41" t="s">
+      <c r="J27" s="35" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="45.75">
-      <c r="A28" s="32">
+      <c r="A28" s="26">
         <v>24</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" s="41" t="s">
+      <c r="C28" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="H28" s="32" t="s">
+      <c r="H28" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I28" s="32" t="s">
+      <c r="I28" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J28" s="41" t="s">
+      <c r="J28" s="35" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="23.25">
-      <c r="A29" s="32">
+      <c r="A29" s="26">
         <v>25</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G29" s="41" t="s">
+      <c r="C29" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H29" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I29" s="32" t="s">
+      <c r="I29" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J29" s="41" t="s">
+      <c r="J29" s="35" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="45.75">
-      <c r="A30" s="32">
+      <c r="A30" s="26">
         <v>26</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G30" s="41" t="s">
+      <c r="C30" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="H30" s="32" t="s">
+      <c r="H30" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I30" s="32" t="s">
+      <c r="I30" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J30" s="41" t="s">
+      <c r="J30" s="35" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="23.25">
-      <c r="A31" s="32">
+      <c r="A31" s="26">
         <v>27</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G31" s="41" t="s">
+      <c r="C31" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="H31" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I31" s="32" t="s">
+      <c r="I31" s="26" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="45.75">
-      <c r="A32" s="32">
+      <c r="A32" s="26">
         <v>28</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="G32" s="43" t="s">
+      <c r="C32" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="H32" s="32" t="s">
+      <c r="H32" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I32" s="32" t="s">
+      <c r="I32" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="J32" s="32" t="s">
+      <c r="J32" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="23.25">
-      <c r="A33" s="32">
+    <row r="33" spans="1:10" ht="45.75">
+      <c r="A33" s="26">
         <v>29</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C33" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="G33" s="41" t="s">
+      <c r="C33" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="H33" s="32" t="s">
+      <c r="J33" s="26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="23.25">
+      <c r="A34" s="26">
+        <v>30</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="H34" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="I33" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="J33" s="32" t="s">
-        <v>135</v>
+      <c r="I34" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="23.25">
+      <c r="A35" s="26">
+        <v>31</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="J35" s="26" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feature] Adaptive Cruise Control - Added signals for IC visualization - trello card: https://trello.com/c/9zKcZxeF/2-feature-adaptive-cruise-control
</commit_message>
<xml_diff>
--- a/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
+++ b/UniDebAutomatedCar/doc/CommunicationMatrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Version &amp; History" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="155">
   <si>
     <t>Change history</t>
   </si>
@@ -660,6 +660,55 @@
   <si>
     <t>DECREMENT: 0
 INCREMENT: 1</t>
+  </si>
+  <si>
+    <t>ACC current cruise control speed</t>
+  </si>
+  <si>
+    <t>ACC current safe distance</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>120.0</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>V3.1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ACC current cruise control speed (ID 32)
+ACC current safe distance (ID 33)
+These signals should used by the IC to inform the driver
+Extended ACC status changed signal (ID 29) with logical values</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -962,7 +1011,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1083,6 +1132,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Magyarázó szöveg" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1502,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E25"/>
+  <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1906,6 +1956,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="26" spans="1:5" ht="90">
+      <c r="A26" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:D2"/>
@@ -1917,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK35"/>
+  <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3018,6 +3085,64 @@
       </c>
       <c r="J35" s="26" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="26">
+        <v>32</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H36" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="J36" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="26">
+        <v>33</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="J37" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>